<commit_message>
plantilla solicitud de cambios actualizada
</commit_message>
<xml_diff>
--- a/Organización/Cambios/PTL_Solicitud_Cambios.xlsx
+++ b/Organización/Cambios/PTL_Solicitud_Cambios.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novela\Documents\Qualtop\SOS\Organización\Cambios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="120" windowWidth="15480" windowHeight="8070" tabRatio="663"/>
   </bookViews>
@@ -16,7 +21,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_Toc105495595" localSheetId="0">'Control de Cambios'!#REF!</definedName>
-    <definedName name="_Toc105495596" localSheetId="0">'Control de Cambios'!$B$12</definedName>
+    <definedName name="_Toc105495596" localSheetId="0">'Control de Cambios'!$C$12</definedName>
     <definedName name="_Toc120446010" localSheetId="0">'Control de Cambios'!#REF!</definedName>
     <definedName name="_Toc120446011" localSheetId="0">'Control de Cambios'!#REF!</definedName>
     <definedName name="Busquedas">[1]Parametros!$A$3:$B$15</definedName>
@@ -30,18 +35,17 @@
     <definedName name="Ocupacion">[2]Parámetros!$B$22:$B$23</definedName>
     <definedName name="UEN">[3]Parámetros!$A$1:$A$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>innevo</author>
-    <author>Zepeda</author>
+    <author>Novela</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,95 +53,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Definición de Estados:
-Identificado:</t>
+          <t>Novela:</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> es el estado inicial de la solicitud de cambios.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Cancelado:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> estado que demuestra que el cliente o el CCC  no quizo implementar el cambio.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>En Implementación:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> estado que denota la aprobación del CCC para la implementación del cambio.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Rechazado: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">estado que denota el rechazo de la implementación del cambio por parte del Cliente o el CCC.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Aprobado (Cerrado)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="1">
-      <text>
         <r>
           <rPr>
             <sz val="9"/>
@@ -145,7 +64,56 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Motivo por el cual se esta realizando el cambio, por ejemplo por parte del cliente o agente interno de la empresa</t>
+          <t xml:space="preserve">
+Responsable</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Novela:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Horas estimadas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Novela:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+$ Costo</t>
         </r>
       </text>
     </comment>
@@ -154,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Datos Generales</t>
   </si>
@@ -237,15 +205,9 @@
     <t>Entregables afectados</t>
   </si>
   <si>
-    <t>Fecha Planeada</t>
-  </si>
-  <si>
     <t>Se incorpora el cambio, el costo lo absorbe la empresa y no hay cambio en fecha de entrega</t>
   </si>
   <si>
-    <t>Fecha Real</t>
-  </si>
-  <si>
     <t>Esfuerzo Estimado</t>
   </si>
   <si>
@@ -268,6 +230,15 @@
   </si>
   <si>
     <t>Costo Estimado</t>
+  </si>
+  <si>
+    <t>Fecha Planeada de inicio</t>
+  </si>
+  <si>
+    <t>Fecha Real de inicio</t>
+  </si>
+  <si>
+    <t>Resp.</t>
   </si>
 </sst>
 </file>
@@ -279,7 +250,7 @@
     <numFmt numFmtId="164" formatCode="mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -407,19 +378,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color indexed="9"/>
       <name val="Calibri"/>
@@ -469,6 +427,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -797,21 +762,15 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -824,50 +783,21 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -875,13 +805,9 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -894,168 +820,133 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="45" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="11" xfId="84" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="11" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="84" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="11" xfId="84" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" xfId="45" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="11" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" xfId="84" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="11" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="11" xfId="84" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="23" fillId="0" borderId="11" xfId="87" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="1"/>
     <cellStyle name="20% - Accent2" xfId="2"/>
     <cellStyle name="20% - Accent3" xfId="3"/>
     <cellStyle name="20% - Accent4" xfId="4"/>
     <cellStyle name="20% - Accent5" xfId="5"/>
     <cellStyle name="20% - Accent6" xfId="6"/>
-    <cellStyle name="20% - Énfasis1" xfId="7" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="8" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="9" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="10" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="11" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="12" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="13"/>
-    <cellStyle name="40% - Accent2" xfId="14"/>
-    <cellStyle name="40% - Accent3" xfId="15"/>
-    <cellStyle name="40% - Accent4" xfId="16"/>
-    <cellStyle name="40% - Accent5" xfId="17"/>
-    <cellStyle name="40% - Accent6" xfId="18"/>
-    <cellStyle name="40% - Énfasis1" xfId="19" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="20" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="21" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="22" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="23" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="24" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="25"/>
-    <cellStyle name="60% - Accent2" xfId="26"/>
-    <cellStyle name="60% - Accent3" xfId="27"/>
-    <cellStyle name="60% - Accent4" xfId="28"/>
-    <cellStyle name="60% - Accent5" xfId="29"/>
-    <cellStyle name="60% - Accent6" xfId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="31" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="32" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="33" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="34" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="35" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="36" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="37"/>
-    <cellStyle name="Accent2" xfId="38"/>
-    <cellStyle name="Accent3" xfId="39"/>
-    <cellStyle name="Accent4" xfId="40"/>
-    <cellStyle name="Accent5" xfId="41"/>
-    <cellStyle name="Accent6" xfId="42"/>
-    <cellStyle name="Bad" xfId="43"/>
-    <cellStyle name="Buena" xfId="44" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="45"/>
-    <cellStyle name="Cálculo" xfId="46" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="47" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="48" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="49"/>
-    <cellStyle name="Encabezado 4" xfId="50" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="51" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="52" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="53" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="54" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="55" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="56" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="57" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Euro" xfId="86"/>
-    <cellStyle name="Explanatory Text" xfId="58"/>
-    <cellStyle name="Good" xfId="59"/>
-    <cellStyle name="Heading 1" xfId="60"/>
-    <cellStyle name="Heading 2" xfId="61"/>
-    <cellStyle name="Heading 3" xfId="62"/>
-    <cellStyle name="Heading 4" xfId="63"/>
-    <cellStyle name="Incorrecto" xfId="64" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="65"/>
-    <cellStyle name="Linked Cell" xfId="66"/>
-    <cellStyle name="Moneda" xfId="87" builtinId="4"/>
-    <cellStyle name="Moneda 2" xfId="67"/>
-    <cellStyle name="Neutral" xfId="68" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7"/>
+    <cellStyle name="40% - Accent2" xfId="8"/>
+    <cellStyle name="40% - Accent3" xfId="9"/>
+    <cellStyle name="40% - Accent4" xfId="10"/>
+    <cellStyle name="40% - Accent5" xfId="11"/>
+    <cellStyle name="40% - Accent6" xfId="12"/>
+    <cellStyle name="60% - Accent1" xfId="13"/>
+    <cellStyle name="60% - Accent2" xfId="14"/>
+    <cellStyle name="60% - Accent3" xfId="15"/>
+    <cellStyle name="60% - Accent4" xfId="16"/>
+    <cellStyle name="60% - Accent5" xfId="17"/>
+    <cellStyle name="60% - Accent6" xfId="18"/>
+    <cellStyle name="Accent1" xfId="21"/>
+    <cellStyle name="Accent2" xfId="22"/>
+    <cellStyle name="Accent3" xfId="23"/>
+    <cellStyle name="Accent4" xfId="24"/>
+    <cellStyle name="Accent5" xfId="25"/>
+    <cellStyle name="Accent6" xfId="26"/>
+    <cellStyle name="Bad" xfId="29"/>
+    <cellStyle name="Calculation" xfId="19"/>
+    <cellStyle name="Check Cell" xfId="20" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="48" builtinId="4"/>
+    <cellStyle name="Euro" xfId="47"/>
+    <cellStyle name="Explanatory Text" xfId="37"/>
+    <cellStyle name="Good" xfId="27" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="39"/>
+    <cellStyle name="Heading 2" xfId="40"/>
+    <cellStyle name="Heading 3" xfId="41"/>
+    <cellStyle name="Heading 4" xfId="28" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="30" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="31" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Moneda 2" xfId="32"/>
+    <cellStyle name="Neutral" xfId="33" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="83"/>
-    <cellStyle name="Normal 2 2" xfId="85"/>
-    <cellStyle name="Normal 3" xfId="84"/>
-    <cellStyle name="Notas" xfId="69" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="70"/>
-    <cellStyle name="Output" xfId="71"/>
-    <cellStyle name="Porcentual 2" xfId="72"/>
-    <cellStyle name="Salida" xfId="73" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="74" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="75" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="76"/>
-    <cellStyle name="Título" xfId="77" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="78" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="79" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="80" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="81" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="82"/>
+    <cellStyle name="Normal 2" xfId="44"/>
+    <cellStyle name="Normal 2 2" xfId="46"/>
+    <cellStyle name="Normal 3" xfId="45"/>
+    <cellStyle name="Note" xfId="34" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="36"/>
+    <cellStyle name="Porcentual 2" xfId="35"/>
+    <cellStyle name="Title" xfId="38"/>
+    <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1618,716 +1509,709 @@
   <sheetPr codeName="Hoja4">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="79" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="256" width="11.42578125" style="1"/>
-    <col min="257" max="257" width="2.7109375" style="1" customWidth="1"/>
-    <col min="258" max="258" width="28.5703125" style="1" customWidth="1"/>
-    <col min="259" max="259" width="57.42578125" style="1" customWidth="1"/>
-    <col min="260" max="512" width="11.42578125" style="1"/>
-    <col min="513" max="513" width="2.7109375" style="1" customWidth="1"/>
-    <col min="514" max="514" width="28.5703125" style="1" customWidth="1"/>
-    <col min="515" max="515" width="57.42578125" style="1" customWidth="1"/>
-    <col min="516" max="768" width="11.42578125" style="1"/>
-    <col min="769" max="769" width="2.7109375" style="1" customWidth="1"/>
-    <col min="770" max="770" width="28.5703125" style="1" customWidth="1"/>
-    <col min="771" max="771" width="57.42578125" style="1" customWidth="1"/>
-    <col min="772" max="1024" width="11.42578125" style="1"/>
-    <col min="1025" max="1025" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="28.5703125" style="1" customWidth="1"/>
-    <col min="1027" max="1027" width="57.42578125" style="1" customWidth="1"/>
-    <col min="1028" max="1280" width="11.42578125" style="1"/>
-    <col min="1281" max="1281" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="28.5703125" style="1" customWidth="1"/>
-    <col min="1283" max="1283" width="57.42578125" style="1" customWidth="1"/>
-    <col min="1284" max="1536" width="11.42578125" style="1"/>
-    <col min="1537" max="1537" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="28.5703125" style="1" customWidth="1"/>
-    <col min="1539" max="1539" width="57.42578125" style="1" customWidth="1"/>
-    <col min="1540" max="1792" width="11.42578125" style="1"/>
-    <col min="1793" max="1793" width="2.7109375" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="28.5703125" style="1" customWidth="1"/>
-    <col min="1795" max="1795" width="57.42578125" style="1" customWidth="1"/>
-    <col min="1796" max="2048" width="11.42578125" style="1"/>
-    <col min="2049" max="2049" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2051" max="2051" width="57.42578125" style="1" customWidth="1"/>
-    <col min="2052" max="2304" width="11.42578125" style="1"/>
-    <col min="2305" max="2305" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2307" max="2307" width="57.42578125" style="1" customWidth="1"/>
-    <col min="2308" max="2560" width="11.42578125" style="1"/>
-    <col min="2561" max="2561" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2563" max="2563" width="57.42578125" style="1" customWidth="1"/>
-    <col min="2564" max="2816" width="11.42578125" style="1"/>
-    <col min="2817" max="2817" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="28.5703125" style="1" customWidth="1"/>
-    <col min="2819" max="2819" width="57.42578125" style="1" customWidth="1"/>
-    <col min="2820" max="3072" width="11.42578125" style="1"/>
-    <col min="3073" max="3073" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3075" max="3075" width="57.42578125" style="1" customWidth="1"/>
-    <col min="3076" max="3328" width="11.42578125" style="1"/>
-    <col min="3329" max="3329" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3331" max="3331" width="57.42578125" style="1" customWidth="1"/>
-    <col min="3332" max="3584" width="11.42578125" style="1"/>
-    <col min="3585" max="3585" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3587" max="3587" width="57.42578125" style="1" customWidth="1"/>
-    <col min="3588" max="3840" width="11.42578125" style="1"/>
-    <col min="3841" max="3841" width="2.7109375" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3843" max="3843" width="57.42578125" style="1" customWidth="1"/>
-    <col min="3844" max="4096" width="11.42578125" style="1"/>
-    <col min="4097" max="4097" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="28.5703125" style="1" customWidth="1"/>
-    <col min="4099" max="4099" width="57.42578125" style="1" customWidth="1"/>
-    <col min="4100" max="4352" width="11.42578125" style="1"/>
-    <col min="4353" max="4353" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="28.5703125" style="1" customWidth="1"/>
-    <col min="4355" max="4355" width="57.42578125" style="1" customWidth="1"/>
-    <col min="4356" max="4608" width="11.42578125" style="1"/>
-    <col min="4609" max="4609" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="28.5703125" style="1" customWidth="1"/>
-    <col min="4611" max="4611" width="57.42578125" style="1" customWidth="1"/>
-    <col min="4612" max="4864" width="11.42578125" style="1"/>
-    <col min="4865" max="4865" width="2.7109375" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="28.5703125" style="1" customWidth="1"/>
-    <col min="4867" max="4867" width="57.42578125" style="1" customWidth="1"/>
-    <col min="4868" max="5120" width="11.42578125" style="1"/>
-    <col min="5121" max="5121" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="28.5703125" style="1" customWidth="1"/>
-    <col min="5123" max="5123" width="57.42578125" style="1" customWidth="1"/>
-    <col min="5124" max="5376" width="11.42578125" style="1"/>
-    <col min="5377" max="5377" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="28.5703125" style="1" customWidth="1"/>
-    <col min="5379" max="5379" width="57.42578125" style="1" customWidth="1"/>
-    <col min="5380" max="5632" width="11.42578125" style="1"/>
-    <col min="5633" max="5633" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="28.5703125" style="1" customWidth="1"/>
-    <col min="5635" max="5635" width="57.42578125" style="1" customWidth="1"/>
-    <col min="5636" max="5888" width="11.42578125" style="1"/>
-    <col min="5889" max="5889" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="28.5703125" style="1" customWidth="1"/>
-    <col min="5891" max="5891" width="57.42578125" style="1" customWidth="1"/>
-    <col min="5892" max="6144" width="11.42578125" style="1"/>
-    <col min="6145" max="6145" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="28.5703125" style="1" customWidth="1"/>
-    <col min="6147" max="6147" width="57.42578125" style="1" customWidth="1"/>
-    <col min="6148" max="6400" width="11.42578125" style="1"/>
-    <col min="6401" max="6401" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="28.5703125" style="1" customWidth="1"/>
-    <col min="6403" max="6403" width="57.42578125" style="1" customWidth="1"/>
-    <col min="6404" max="6656" width="11.42578125" style="1"/>
-    <col min="6657" max="6657" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="28.5703125" style="1" customWidth="1"/>
-    <col min="6659" max="6659" width="57.42578125" style="1" customWidth="1"/>
-    <col min="6660" max="6912" width="11.42578125" style="1"/>
-    <col min="6913" max="6913" width="2.7109375" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="28.5703125" style="1" customWidth="1"/>
-    <col min="6915" max="6915" width="57.42578125" style="1" customWidth="1"/>
-    <col min="6916" max="7168" width="11.42578125" style="1"/>
-    <col min="7169" max="7169" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7171" max="7171" width="57.42578125" style="1" customWidth="1"/>
-    <col min="7172" max="7424" width="11.42578125" style="1"/>
-    <col min="7425" max="7425" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7427" max="7427" width="57.42578125" style="1" customWidth="1"/>
-    <col min="7428" max="7680" width="11.42578125" style="1"/>
-    <col min="7681" max="7681" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7683" max="7683" width="57.42578125" style="1" customWidth="1"/>
-    <col min="7684" max="7936" width="11.42578125" style="1"/>
-    <col min="7937" max="7937" width="2.7109375" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="28.5703125" style="1" customWidth="1"/>
-    <col min="7939" max="7939" width="57.42578125" style="1" customWidth="1"/>
-    <col min="7940" max="8192" width="11.42578125" style="1"/>
-    <col min="8193" max="8193" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8195" max="8195" width="57.42578125" style="1" customWidth="1"/>
-    <col min="8196" max="8448" width="11.42578125" style="1"/>
-    <col min="8449" max="8449" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8451" max="8451" width="57.42578125" style="1" customWidth="1"/>
-    <col min="8452" max="8704" width="11.42578125" style="1"/>
-    <col min="8705" max="8705" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8707" max="8707" width="57.42578125" style="1" customWidth="1"/>
-    <col min="8708" max="8960" width="11.42578125" style="1"/>
-    <col min="8961" max="8961" width="2.7109375" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8963" max="8963" width="57.42578125" style="1" customWidth="1"/>
-    <col min="8964" max="9216" width="11.42578125" style="1"/>
-    <col min="9217" max="9217" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="28.5703125" style="1" customWidth="1"/>
-    <col min="9219" max="9219" width="57.42578125" style="1" customWidth="1"/>
-    <col min="9220" max="9472" width="11.42578125" style="1"/>
-    <col min="9473" max="9473" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="28.5703125" style="1" customWidth="1"/>
-    <col min="9475" max="9475" width="57.42578125" style="1" customWidth="1"/>
-    <col min="9476" max="9728" width="11.42578125" style="1"/>
-    <col min="9729" max="9729" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="28.5703125" style="1" customWidth="1"/>
-    <col min="9731" max="9731" width="57.42578125" style="1" customWidth="1"/>
-    <col min="9732" max="9984" width="11.42578125" style="1"/>
-    <col min="9985" max="9985" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="28.5703125" style="1" customWidth="1"/>
-    <col min="9987" max="9987" width="57.42578125" style="1" customWidth="1"/>
-    <col min="9988" max="10240" width="11.42578125" style="1"/>
-    <col min="10241" max="10241" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="28.5703125" style="1" customWidth="1"/>
-    <col min="10243" max="10243" width="57.42578125" style="1" customWidth="1"/>
-    <col min="10244" max="10496" width="11.42578125" style="1"/>
-    <col min="10497" max="10497" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="28.5703125" style="1" customWidth="1"/>
-    <col min="10499" max="10499" width="57.42578125" style="1" customWidth="1"/>
-    <col min="10500" max="10752" width="11.42578125" style="1"/>
-    <col min="10753" max="10753" width="2.7109375" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="28.5703125" style="1" customWidth="1"/>
-    <col min="10755" max="10755" width="57.42578125" style="1" customWidth="1"/>
-    <col min="10756" max="11008" width="11.42578125" style="1"/>
-    <col min="11009" max="11009" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="28.5703125" style="1" customWidth="1"/>
-    <col min="11011" max="11011" width="57.42578125" style="1" customWidth="1"/>
-    <col min="11012" max="11264" width="11.42578125" style="1"/>
-    <col min="11265" max="11265" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="28.5703125" style="1" customWidth="1"/>
-    <col min="11267" max="11267" width="57.42578125" style="1" customWidth="1"/>
-    <col min="11268" max="11520" width="11.42578125" style="1"/>
-    <col min="11521" max="11521" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="28.5703125" style="1" customWidth="1"/>
-    <col min="11523" max="11523" width="57.42578125" style="1" customWidth="1"/>
-    <col min="11524" max="11776" width="11.42578125" style="1"/>
-    <col min="11777" max="11777" width="2.7109375" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="28.5703125" style="1" customWidth="1"/>
-    <col min="11779" max="11779" width="57.42578125" style="1" customWidth="1"/>
-    <col min="11780" max="12032" width="11.42578125" style="1"/>
-    <col min="12033" max="12033" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="28.5703125" style="1" customWidth="1"/>
-    <col min="12035" max="12035" width="57.42578125" style="1" customWidth="1"/>
-    <col min="12036" max="12288" width="11.42578125" style="1"/>
-    <col min="12289" max="12289" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="28.5703125" style="1" customWidth="1"/>
-    <col min="12291" max="12291" width="57.42578125" style="1" customWidth="1"/>
-    <col min="12292" max="12544" width="11.42578125" style="1"/>
-    <col min="12545" max="12545" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="28.5703125" style="1" customWidth="1"/>
-    <col min="12547" max="12547" width="57.42578125" style="1" customWidth="1"/>
-    <col min="12548" max="12800" width="11.42578125" style="1"/>
-    <col min="12801" max="12801" width="2.7109375" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="28.5703125" style="1" customWidth="1"/>
-    <col min="12803" max="12803" width="57.42578125" style="1" customWidth="1"/>
-    <col min="12804" max="13056" width="11.42578125" style="1"/>
-    <col min="13057" max="13057" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="28.5703125" style="1" customWidth="1"/>
-    <col min="13059" max="13059" width="57.42578125" style="1" customWidth="1"/>
-    <col min="13060" max="13312" width="11.42578125" style="1"/>
-    <col min="13313" max="13313" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="28.5703125" style="1" customWidth="1"/>
-    <col min="13315" max="13315" width="57.42578125" style="1" customWidth="1"/>
-    <col min="13316" max="13568" width="11.42578125" style="1"/>
-    <col min="13569" max="13569" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="28.5703125" style="1" customWidth="1"/>
-    <col min="13571" max="13571" width="57.42578125" style="1" customWidth="1"/>
-    <col min="13572" max="13824" width="11.42578125" style="1"/>
-    <col min="13825" max="13825" width="2.7109375" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="28.5703125" style="1" customWidth="1"/>
-    <col min="13827" max="13827" width="57.42578125" style="1" customWidth="1"/>
-    <col min="13828" max="14080" width="11.42578125" style="1"/>
-    <col min="14081" max="14081" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="28.5703125" style="1" customWidth="1"/>
-    <col min="14083" max="14083" width="57.42578125" style="1" customWidth="1"/>
-    <col min="14084" max="14336" width="11.42578125" style="1"/>
-    <col min="14337" max="14337" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="28.5703125" style="1" customWidth="1"/>
-    <col min="14339" max="14339" width="57.42578125" style="1" customWidth="1"/>
-    <col min="14340" max="14592" width="11.42578125" style="1"/>
-    <col min="14593" max="14593" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="28.5703125" style="1" customWidth="1"/>
-    <col min="14595" max="14595" width="57.42578125" style="1" customWidth="1"/>
-    <col min="14596" max="14848" width="11.42578125" style="1"/>
-    <col min="14849" max="14849" width="2.7109375" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="28.5703125" style="1" customWidth="1"/>
-    <col min="14851" max="14851" width="57.42578125" style="1" customWidth="1"/>
-    <col min="14852" max="15104" width="11.42578125" style="1"/>
-    <col min="15105" max="15105" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="28.5703125" style="1" customWidth="1"/>
-    <col min="15107" max="15107" width="57.42578125" style="1" customWidth="1"/>
-    <col min="15108" max="15360" width="11.42578125" style="1"/>
-    <col min="15361" max="15361" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="28.5703125" style="1" customWidth="1"/>
-    <col min="15363" max="15363" width="57.42578125" style="1" customWidth="1"/>
-    <col min="15364" max="15616" width="11.42578125" style="1"/>
-    <col min="15617" max="15617" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="28.5703125" style="1" customWidth="1"/>
-    <col min="15619" max="15619" width="57.42578125" style="1" customWidth="1"/>
-    <col min="15620" max="15872" width="11.42578125" style="1"/>
-    <col min="15873" max="15873" width="2.7109375" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="28.5703125" style="1" customWidth="1"/>
-    <col min="15875" max="15875" width="57.42578125" style="1" customWidth="1"/>
-    <col min="15876" max="16128" width="11.42578125" style="1"/>
-    <col min="16129" max="16129" width="2.7109375" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="28.5703125" style="1" customWidth="1"/>
-    <col min="16131" max="16131" width="57.42578125" style="1" customWidth="1"/>
-    <col min="16132" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="2.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="88.42578125" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="7" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="7"/>
+    <col min="11" max="11" width="2.140625" style="7" customWidth="1"/>
+    <col min="12" max="257" width="11.42578125" style="7"/>
+    <col min="258" max="258" width="2.7109375" style="7" customWidth="1"/>
+    <col min="259" max="259" width="28.5703125" style="7" customWidth="1"/>
+    <col min="260" max="260" width="57.42578125" style="7" customWidth="1"/>
+    <col min="261" max="513" width="11.42578125" style="7"/>
+    <col min="514" max="514" width="2.7109375" style="7" customWidth="1"/>
+    <col min="515" max="515" width="28.5703125" style="7" customWidth="1"/>
+    <col min="516" max="516" width="57.42578125" style="7" customWidth="1"/>
+    <col min="517" max="769" width="11.42578125" style="7"/>
+    <col min="770" max="770" width="2.7109375" style="7" customWidth="1"/>
+    <col min="771" max="771" width="28.5703125" style="7" customWidth="1"/>
+    <col min="772" max="772" width="57.42578125" style="7" customWidth="1"/>
+    <col min="773" max="1025" width="11.42578125" style="7"/>
+    <col min="1026" max="1026" width="2.7109375" style="7" customWidth="1"/>
+    <col min="1027" max="1027" width="28.5703125" style="7" customWidth="1"/>
+    <col min="1028" max="1028" width="57.42578125" style="7" customWidth="1"/>
+    <col min="1029" max="1281" width="11.42578125" style="7"/>
+    <col min="1282" max="1282" width="2.7109375" style="7" customWidth="1"/>
+    <col min="1283" max="1283" width="28.5703125" style="7" customWidth="1"/>
+    <col min="1284" max="1284" width="57.42578125" style="7" customWidth="1"/>
+    <col min="1285" max="1537" width="11.42578125" style="7"/>
+    <col min="1538" max="1538" width="2.7109375" style="7" customWidth="1"/>
+    <col min="1539" max="1539" width="28.5703125" style="7" customWidth="1"/>
+    <col min="1540" max="1540" width="57.42578125" style="7" customWidth="1"/>
+    <col min="1541" max="1793" width="11.42578125" style="7"/>
+    <col min="1794" max="1794" width="2.7109375" style="7" customWidth="1"/>
+    <col min="1795" max="1795" width="28.5703125" style="7" customWidth="1"/>
+    <col min="1796" max="1796" width="57.42578125" style="7" customWidth="1"/>
+    <col min="1797" max="2049" width="11.42578125" style="7"/>
+    <col min="2050" max="2050" width="2.7109375" style="7" customWidth="1"/>
+    <col min="2051" max="2051" width="28.5703125" style="7" customWidth="1"/>
+    <col min="2052" max="2052" width="57.42578125" style="7" customWidth="1"/>
+    <col min="2053" max="2305" width="11.42578125" style="7"/>
+    <col min="2306" max="2306" width="2.7109375" style="7" customWidth="1"/>
+    <col min="2307" max="2307" width="28.5703125" style="7" customWidth="1"/>
+    <col min="2308" max="2308" width="57.42578125" style="7" customWidth="1"/>
+    <col min="2309" max="2561" width="11.42578125" style="7"/>
+    <col min="2562" max="2562" width="2.7109375" style="7" customWidth="1"/>
+    <col min="2563" max="2563" width="28.5703125" style="7" customWidth="1"/>
+    <col min="2564" max="2564" width="57.42578125" style="7" customWidth="1"/>
+    <col min="2565" max="2817" width="11.42578125" style="7"/>
+    <col min="2818" max="2818" width="2.7109375" style="7" customWidth="1"/>
+    <col min="2819" max="2819" width="28.5703125" style="7" customWidth="1"/>
+    <col min="2820" max="2820" width="57.42578125" style="7" customWidth="1"/>
+    <col min="2821" max="3073" width="11.42578125" style="7"/>
+    <col min="3074" max="3074" width="2.7109375" style="7" customWidth="1"/>
+    <col min="3075" max="3075" width="28.5703125" style="7" customWidth="1"/>
+    <col min="3076" max="3076" width="57.42578125" style="7" customWidth="1"/>
+    <col min="3077" max="3329" width="11.42578125" style="7"/>
+    <col min="3330" max="3330" width="2.7109375" style="7" customWidth="1"/>
+    <col min="3331" max="3331" width="28.5703125" style="7" customWidth="1"/>
+    <col min="3332" max="3332" width="57.42578125" style="7" customWidth="1"/>
+    <col min="3333" max="3585" width="11.42578125" style="7"/>
+    <col min="3586" max="3586" width="2.7109375" style="7" customWidth="1"/>
+    <col min="3587" max="3587" width="28.5703125" style="7" customWidth="1"/>
+    <col min="3588" max="3588" width="57.42578125" style="7" customWidth="1"/>
+    <col min="3589" max="3841" width="11.42578125" style="7"/>
+    <col min="3842" max="3842" width="2.7109375" style="7" customWidth="1"/>
+    <col min="3843" max="3843" width="28.5703125" style="7" customWidth="1"/>
+    <col min="3844" max="3844" width="57.42578125" style="7" customWidth="1"/>
+    <col min="3845" max="4097" width="11.42578125" style="7"/>
+    <col min="4098" max="4098" width="2.7109375" style="7" customWidth="1"/>
+    <col min="4099" max="4099" width="28.5703125" style="7" customWidth="1"/>
+    <col min="4100" max="4100" width="57.42578125" style="7" customWidth="1"/>
+    <col min="4101" max="4353" width="11.42578125" style="7"/>
+    <col min="4354" max="4354" width="2.7109375" style="7" customWidth="1"/>
+    <col min="4355" max="4355" width="28.5703125" style="7" customWidth="1"/>
+    <col min="4356" max="4356" width="57.42578125" style="7" customWidth="1"/>
+    <col min="4357" max="4609" width="11.42578125" style="7"/>
+    <col min="4610" max="4610" width="2.7109375" style="7" customWidth="1"/>
+    <col min="4611" max="4611" width="28.5703125" style="7" customWidth="1"/>
+    <col min="4612" max="4612" width="57.42578125" style="7" customWidth="1"/>
+    <col min="4613" max="4865" width="11.42578125" style="7"/>
+    <col min="4866" max="4866" width="2.7109375" style="7" customWidth="1"/>
+    <col min="4867" max="4867" width="28.5703125" style="7" customWidth="1"/>
+    <col min="4868" max="4868" width="57.42578125" style="7" customWidth="1"/>
+    <col min="4869" max="5121" width="11.42578125" style="7"/>
+    <col min="5122" max="5122" width="2.7109375" style="7" customWidth="1"/>
+    <col min="5123" max="5123" width="28.5703125" style="7" customWidth="1"/>
+    <col min="5124" max="5124" width="57.42578125" style="7" customWidth="1"/>
+    <col min="5125" max="5377" width="11.42578125" style="7"/>
+    <col min="5378" max="5378" width="2.7109375" style="7" customWidth="1"/>
+    <col min="5379" max="5379" width="28.5703125" style="7" customWidth="1"/>
+    <col min="5380" max="5380" width="57.42578125" style="7" customWidth="1"/>
+    <col min="5381" max="5633" width="11.42578125" style="7"/>
+    <col min="5634" max="5634" width="2.7109375" style="7" customWidth="1"/>
+    <col min="5635" max="5635" width="28.5703125" style="7" customWidth="1"/>
+    <col min="5636" max="5636" width="57.42578125" style="7" customWidth="1"/>
+    <col min="5637" max="5889" width="11.42578125" style="7"/>
+    <col min="5890" max="5890" width="2.7109375" style="7" customWidth="1"/>
+    <col min="5891" max="5891" width="28.5703125" style="7" customWidth="1"/>
+    <col min="5892" max="5892" width="57.42578125" style="7" customWidth="1"/>
+    <col min="5893" max="6145" width="11.42578125" style="7"/>
+    <col min="6146" max="6146" width="2.7109375" style="7" customWidth="1"/>
+    <col min="6147" max="6147" width="28.5703125" style="7" customWidth="1"/>
+    <col min="6148" max="6148" width="57.42578125" style="7" customWidth="1"/>
+    <col min="6149" max="6401" width="11.42578125" style="7"/>
+    <col min="6402" max="6402" width="2.7109375" style="7" customWidth="1"/>
+    <col min="6403" max="6403" width="28.5703125" style="7" customWidth="1"/>
+    <col min="6404" max="6404" width="57.42578125" style="7" customWidth="1"/>
+    <col min="6405" max="6657" width="11.42578125" style="7"/>
+    <col min="6658" max="6658" width="2.7109375" style="7" customWidth="1"/>
+    <col min="6659" max="6659" width="28.5703125" style="7" customWidth="1"/>
+    <col min="6660" max="6660" width="57.42578125" style="7" customWidth="1"/>
+    <col min="6661" max="6913" width="11.42578125" style="7"/>
+    <col min="6914" max="6914" width="2.7109375" style="7" customWidth="1"/>
+    <col min="6915" max="6915" width="28.5703125" style="7" customWidth="1"/>
+    <col min="6916" max="6916" width="57.42578125" style="7" customWidth="1"/>
+    <col min="6917" max="7169" width="11.42578125" style="7"/>
+    <col min="7170" max="7170" width="2.7109375" style="7" customWidth="1"/>
+    <col min="7171" max="7171" width="28.5703125" style="7" customWidth="1"/>
+    <col min="7172" max="7172" width="57.42578125" style="7" customWidth="1"/>
+    <col min="7173" max="7425" width="11.42578125" style="7"/>
+    <col min="7426" max="7426" width="2.7109375" style="7" customWidth="1"/>
+    <col min="7427" max="7427" width="28.5703125" style="7" customWidth="1"/>
+    <col min="7428" max="7428" width="57.42578125" style="7" customWidth="1"/>
+    <col min="7429" max="7681" width="11.42578125" style="7"/>
+    <col min="7682" max="7682" width="2.7109375" style="7" customWidth="1"/>
+    <col min="7683" max="7683" width="28.5703125" style="7" customWidth="1"/>
+    <col min="7684" max="7684" width="57.42578125" style="7" customWidth="1"/>
+    <col min="7685" max="7937" width="11.42578125" style="7"/>
+    <col min="7938" max="7938" width="2.7109375" style="7" customWidth="1"/>
+    <col min="7939" max="7939" width="28.5703125" style="7" customWidth="1"/>
+    <col min="7940" max="7940" width="57.42578125" style="7" customWidth="1"/>
+    <col min="7941" max="8193" width="11.42578125" style="7"/>
+    <col min="8194" max="8194" width="2.7109375" style="7" customWidth="1"/>
+    <col min="8195" max="8195" width="28.5703125" style="7" customWidth="1"/>
+    <col min="8196" max="8196" width="57.42578125" style="7" customWidth="1"/>
+    <col min="8197" max="8449" width="11.42578125" style="7"/>
+    <col min="8450" max="8450" width="2.7109375" style="7" customWidth="1"/>
+    <col min="8451" max="8451" width="28.5703125" style="7" customWidth="1"/>
+    <col min="8452" max="8452" width="57.42578125" style="7" customWidth="1"/>
+    <col min="8453" max="8705" width="11.42578125" style="7"/>
+    <col min="8706" max="8706" width="2.7109375" style="7" customWidth="1"/>
+    <col min="8707" max="8707" width="28.5703125" style="7" customWidth="1"/>
+    <col min="8708" max="8708" width="57.42578125" style="7" customWidth="1"/>
+    <col min="8709" max="8961" width="11.42578125" style="7"/>
+    <col min="8962" max="8962" width="2.7109375" style="7" customWidth="1"/>
+    <col min="8963" max="8963" width="28.5703125" style="7" customWidth="1"/>
+    <col min="8964" max="8964" width="57.42578125" style="7" customWidth="1"/>
+    <col min="8965" max="9217" width="11.42578125" style="7"/>
+    <col min="9218" max="9218" width="2.7109375" style="7" customWidth="1"/>
+    <col min="9219" max="9219" width="28.5703125" style="7" customWidth="1"/>
+    <col min="9220" max="9220" width="57.42578125" style="7" customWidth="1"/>
+    <col min="9221" max="9473" width="11.42578125" style="7"/>
+    <col min="9474" max="9474" width="2.7109375" style="7" customWidth="1"/>
+    <col min="9475" max="9475" width="28.5703125" style="7" customWidth="1"/>
+    <col min="9476" max="9476" width="57.42578125" style="7" customWidth="1"/>
+    <col min="9477" max="9729" width="11.42578125" style="7"/>
+    <col min="9730" max="9730" width="2.7109375" style="7" customWidth="1"/>
+    <col min="9731" max="9731" width="28.5703125" style="7" customWidth="1"/>
+    <col min="9732" max="9732" width="57.42578125" style="7" customWidth="1"/>
+    <col min="9733" max="9985" width="11.42578125" style="7"/>
+    <col min="9986" max="9986" width="2.7109375" style="7" customWidth="1"/>
+    <col min="9987" max="9987" width="28.5703125" style="7" customWidth="1"/>
+    <col min="9988" max="9988" width="57.42578125" style="7" customWidth="1"/>
+    <col min="9989" max="10241" width="11.42578125" style="7"/>
+    <col min="10242" max="10242" width="2.7109375" style="7" customWidth="1"/>
+    <col min="10243" max="10243" width="28.5703125" style="7" customWidth="1"/>
+    <col min="10244" max="10244" width="57.42578125" style="7" customWidth="1"/>
+    <col min="10245" max="10497" width="11.42578125" style="7"/>
+    <col min="10498" max="10498" width="2.7109375" style="7" customWidth="1"/>
+    <col min="10499" max="10499" width="28.5703125" style="7" customWidth="1"/>
+    <col min="10500" max="10500" width="57.42578125" style="7" customWidth="1"/>
+    <col min="10501" max="10753" width="11.42578125" style="7"/>
+    <col min="10754" max="10754" width="2.7109375" style="7" customWidth="1"/>
+    <col min="10755" max="10755" width="28.5703125" style="7" customWidth="1"/>
+    <col min="10756" max="10756" width="57.42578125" style="7" customWidth="1"/>
+    <col min="10757" max="11009" width="11.42578125" style="7"/>
+    <col min="11010" max="11010" width="2.7109375" style="7" customWidth="1"/>
+    <col min="11011" max="11011" width="28.5703125" style="7" customWidth="1"/>
+    <col min="11012" max="11012" width="57.42578125" style="7" customWidth="1"/>
+    <col min="11013" max="11265" width="11.42578125" style="7"/>
+    <col min="11266" max="11266" width="2.7109375" style="7" customWidth="1"/>
+    <col min="11267" max="11267" width="28.5703125" style="7" customWidth="1"/>
+    <col min="11268" max="11268" width="57.42578125" style="7" customWidth="1"/>
+    <col min="11269" max="11521" width="11.42578125" style="7"/>
+    <col min="11522" max="11522" width="2.7109375" style="7" customWidth="1"/>
+    <col min="11523" max="11523" width="28.5703125" style="7" customWidth="1"/>
+    <col min="11524" max="11524" width="57.42578125" style="7" customWidth="1"/>
+    <col min="11525" max="11777" width="11.42578125" style="7"/>
+    <col min="11778" max="11778" width="2.7109375" style="7" customWidth="1"/>
+    <col min="11779" max="11779" width="28.5703125" style="7" customWidth="1"/>
+    <col min="11780" max="11780" width="57.42578125" style="7" customWidth="1"/>
+    <col min="11781" max="12033" width="11.42578125" style="7"/>
+    <col min="12034" max="12034" width="2.7109375" style="7" customWidth="1"/>
+    <col min="12035" max="12035" width="28.5703125" style="7" customWidth="1"/>
+    <col min="12036" max="12036" width="57.42578125" style="7" customWidth="1"/>
+    <col min="12037" max="12289" width="11.42578125" style="7"/>
+    <col min="12290" max="12290" width="2.7109375" style="7" customWidth="1"/>
+    <col min="12291" max="12291" width="28.5703125" style="7" customWidth="1"/>
+    <col min="12292" max="12292" width="57.42578125" style="7" customWidth="1"/>
+    <col min="12293" max="12545" width="11.42578125" style="7"/>
+    <col min="12546" max="12546" width="2.7109375" style="7" customWidth="1"/>
+    <col min="12547" max="12547" width="28.5703125" style="7" customWidth="1"/>
+    <col min="12548" max="12548" width="57.42578125" style="7" customWidth="1"/>
+    <col min="12549" max="12801" width="11.42578125" style="7"/>
+    <col min="12802" max="12802" width="2.7109375" style="7" customWidth="1"/>
+    <col min="12803" max="12803" width="28.5703125" style="7" customWidth="1"/>
+    <col min="12804" max="12804" width="57.42578125" style="7" customWidth="1"/>
+    <col min="12805" max="13057" width="11.42578125" style="7"/>
+    <col min="13058" max="13058" width="2.7109375" style="7" customWidth="1"/>
+    <col min="13059" max="13059" width="28.5703125" style="7" customWidth="1"/>
+    <col min="13060" max="13060" width="57.42578125" style="7" customWidth="1"/>
+    <col min="13061" max="13313" width="11.42578125" style="7"/>
+    <col min="13314" max="13314" width="2.7109375" style="7" customWidth="1"/>
+    <col min="13315" max="13315" width="28.5703125" style="7" customWidth="1"/>
+    <col min="13316" max="13316" width="57.42578125" style="7" customWidth="1"/>
+    <col min="13317" max="13569" width="11.42578125" style="7"/>
+    <col min="13570" max="13570" width="2.7109375" style="7" customWidth="1"/>
+    <col min="13571" max="13571" width="28.5703125" style="7" customWidth="1"/>
+    <col min="13572" max="13572" width="57.42578125" style="7" customWidth="1"/>
+    <col min="13573" max="13825" width="11.42578125" style="7"/>
+    <col min="13826" max="13826" width="2.7109375" style="7" customWidth="1"/>
+    <col min="13827" max="13827" width="28.5703125" style="7" customWidth="1"/>
+    <col min="13828" max="13828" width="57.42578125" style="7" customWidth="1"/>
+    <col min="13829" max="14081" width="11.42578125" style="7"/>
+    <col min="14082" max="14082" width="2.7109375" style="7" customWidth="1"/>
+    <col min="14083" max="14083" width="28.5703125" style="7" customWidth="1"/>
+    <col min="14084" max="14084" width="57.42578125" style="7" customWidth="1"/>
+    <col min="14085" max="14337" width="11.42578125" style="7"/>
+    <col min="14338" max="14338" width="2.7109375" style="7" customWidth="1"/>
+    <col min="14339" max="14339" width="28.5703125" style="7" customWidth="1"/>
+    <col min="14340" max="14340" width="57.42578125" style="7" customWidth="1"/>
+    <col min="14341" max="14593" width="11.42578125" style="7"/>
+    <col min="14594" max="14594" width="2.7109375" style="7" customWidth="1"/>
+    <col min="14595" max="14595" width="28.5703125" style="7" customWidth="1"/>
+    <col min="14596" max="14596" width="57.42578125" style="7" customWidth="1"/>
+    <col min="14597" max="14849" width="11.42578125" style="7"/>
+    <col min="14850" max="14850" width="2.7109375" style="7" customWidth="1"/>
+    <col min="14851" max="14851" width="28.5703125" style="7" customWidth="1"/>
+    <col min="14852" max="14852" width="57.42578125" style="7" customWidth="1"/>
+    <col min="14853" max="15105" width="11.42578125" style="7"/>
+    <col min="15106" max="15106" width="2.7109375" style="7" customWidth="1"/>
+    <col min="15107" max="15107" width="28.5703125" style="7" customWidth="1"/>
+    <col min="15108" max="15108" width="57.42578125" style="7" customWidth="1"/>
+    <col min="15109" max="15361" width="11.42578125" style="7"/>
+    <col min="15362" max="15362" width="2.7109375" style="7" customWidth="1"/>
+    <col min="15363" max="15363" width="28.5703125" style="7" customWidth="1"/>
+    <col min="15364" max="15364" width="57.42578125" style="7" customWidth="1"/>
+    <col min="15365" max="15617" width="11.42578125" style="7"/>
+    <col min="15618" max="15618" width="2.7109375" style="7" customWidth="1"/>
+    <col min="15619" max="15619" width="28.5703125" style="7" customWidth="1"/>
+    <col min="15620" max="15620" width="57.42578125" style="7" customWidth="1"/>
+    <col min="15621" max="15873" width="11.42578125" style="7"/>
+    <col min="15874" max="15874" width="2.7109375" style="7" customWidth="1"/>
+    <col min="15875" max="15875" width="28.5703125" style="7" customWidth="1"/>
+    <col min="15876" max="15876" width="57.42578125" style="7" customWidth="1"/>
+    <col min="15877" max="16129" width="11.42578125" style="7"/>
+    <col min="16130" max="16130" width="2.7109375" style="7" customWidth="1"/>
+    <col min="16131" max="16131" width="28.5703125" style="7" customWidth="1"/>
+    <col min="16132" max="16132" width="57.42578125" style="7" customWidth="1"/>
+    <col min="16133" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="25"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="25"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="25"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="25"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="25"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="25"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="25"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="25"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="25"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="25"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="25"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="16">
+        <f>SUM(I13:I23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-    </row>
-    <row r="28" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="11">
-        <f>SUM(H13:H31)</f>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="24">
+        <f>SUM(J13:J23)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="5"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="20"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="25">
-        <f>SUM(I13:I31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="8" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="8" t="s">
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="8" t="s">
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="8"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="8" t="s">
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="8"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="8" t="s">
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="8"/>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="26" t="s">
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="26"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="8" t="s">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="8"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="8" t="s">
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="8"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="8" t="s">
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C36" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="8"/>
+      <c r="D36" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H2:H6"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="19">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C37">
-      <formula1>$E$2:$E$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29">
+      <formula1>$F$2:$F$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D36">
       <formula1>"Aprobado,Rechazado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10">
       <formula1>"Alta,Media,Baja"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
-      <formula1>$F$2:$F$6</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
+      <formula1>$G$2:$G$6</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -2411,15 +2295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -2436,6 +2311,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9B730C3-1047-4794-B798-57186B6BC346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2448,14 +2331,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>